<commit_message>
Made event timeline compatible with db entries.
</commit_message>
<xml_diff>
--- a/TilerElements/migrationStatus.xlsx
+++ b/TilerElements/migrationStatus.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerom\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerom\Documents\Visual Studio 2015\Projects\WagTap\My24HourTimerWPF\TilerElements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="0" windowWidth="56175" windowHeight="28995"/>
+    <workbookView xWindow="4275" yWindow="0" windowWidth="56175" windowHeight="28995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="59">
   <si>
     <t>BlobSubCalendarEvent.cs</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>undoable</t>
+  </si>
+  <si>
+    <t>migrated</t>
   </si>
 </sst>
 </file>
@@ -547,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H11:J67"/>
+  <dimension ref="H10:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,6 +564,14 @@
     <col min="8" max="8" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="10" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="11" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
         <v>0</v>
@@ -573,6 +587,12 @@
       <c r="H12" t="s">
         <v>1</v>
       </c>
+      <c r="I12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="13" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
@@ -639,6 +659,12 @@
     <row r="23" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
         <v>11</v>
+      </c>
+      <c r="I23" t="s">
+        <v>56</v>
+      </c>
+      <c r="J23" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="8:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added some extra modifications to allow for different instance
</commit_message>
<xml_diff>
--- a/TilerElements/migrationStatus.xlsx
+++ b/TilerElements/migrationStatus.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="0" windowWidth="56175" windowHeight="28995"/>
+    <workbookView xWindow="6135" yWindow="0" windowWidth="56175" windowHeight="28995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
   <si>
     <t>BlobSubCalendarEvent.cs</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>EventID.cs</t>
-  </si>
-  <si>
-    <t>EventIDGenerator.cs</t>
   </si>
   <si>
     <t>EventLearn.cs</t>
@@ -553,23 +550,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H10:J67"/>
+  <dimension ref="H10:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="35.140625" customWidth="1"/>
+    <col min="8" max="8" width="35.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="10" spans="8:10" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="8:10" x14ac:dyDescent="0.25">
@@ -577,10 +574,10 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="8:10" x14ac:dyDescent="0.25">
@@ -588,10 +585,10 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="8:10" x14ac:dyDescent="0.25">
@@ -624,7 +621,7 @@
         <v>6</v>
       </c>
       <c r="I18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="8:10" x14ac:dyDescent="0.25">
@@ -632,10 +629,10 @@
         <v>7</v>
       </c>
       <c r="I19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="8:10" x14ac:dyDescent="0.25">
@@ -647,38 +644,41 @@
       <c r="H21" t="s">
         <v>9</v>
       </c>
+      <c r="I21" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="22" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H22" t="s">
         <v>10</v>
       </c>
       <c r="I22" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="J22" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
         <v>11</v>
       </c>
-      <c r="I23" t="s">
-        <v>56</v>
-      </c>
-      <c r="J23" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="24" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
         <v>12</v>
       </c>
+      <c r="I24" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="25" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
         <v>13</v>
       </c>
-      <c r="I25" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="26" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
@@ -689,16 +689,19 @@
       <c r="H27" t="s">
         <v>15</v>
       </c>
+      <c r="I27" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="28" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>16</v>
       </c>
       <c r="I28" t="s">
-        <v>56</v>
-      </c>
-      <c r="J28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="8:10" x14ac:dyDescent="0.25">
@@ -706,7 +709,10 @@
         <v>17</v>
       </c>
       <c r="I29" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="J29" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="8:10" x14ac:dyDescent="0.25">
@@ -714,10 +720,7 @@
         <v>18</v>
       </c>
       <c r="I30" t="s">
-        <v>56</v>
-      </c>
-      <c r="J30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="8:10" x14ac:dyDescent="0.25">
@@ -725,16 +728,13 @@
         <v>19</v>
       </c>
       <c r="I31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H32" t="s">
         <v>20</v>
       </c>
-      <c r="I32" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="33" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
@@ -745,25 +745,25 @@
       <c r="H34" t="s">
         <v>22</v>
       </c>
+      <c r="I34" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="35" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H35" t="s">
         <v>23</v>
       </c>
       <c r="I35" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="J35" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
         <v>24</v>
       </c>
-      <c r="I36" t="s">
-        <v>56</v>
-      </c>
-      <c r="J36" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="37" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H37" t="s">
@@ -779,26 +779,29 @@
       <c r="H39" t="s">
         <v>27</v>
       </c>
+      <c r="I39" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="40" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H40" t="s">
         <v>28</v>
       </c>
-      <c r="I40" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="41" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H41" t="s">
         <v>29</v>
       </c>
+      <c r="I41" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="42" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H42" t="s">
         <v>30</v>
       </c>
       <c r="I42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="8:10" x14ac:dyDescent="0.25">
@@ -806,7 +809,7 @@
         <v>31</v>
       </c>
       <c r="I43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="8:10" x14ac:dyDescent="0.25">
@@ -814,7 +817,7 @@
         <v>32</v>
       </c>
       <c r="I44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="8:10" x14ac:dyDescent="0.25">
@@ -822,16 +825,13 @@
         <v>33</v>
       </c>
       <c r="I45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H46" t="s">
         <v>34</v>
       </c>
-      <c r="I46" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="47" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H47" t="s">
@@ -843,135 +843,130 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H49" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H50" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H51" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H52" t="s">
         <v>40</v>
       </c>
       <c r="I52" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H53" t="s">
         <v>41</v>
       </c>
       <c r="I53" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H54" t="s">
         <v>42</v>
       </c>
       <c r="I54" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H55" t="s">
         <v>43</v>
       </c>
       <c r="I55" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H56" t="s">
         <v>44</v>
       </c>
       <c r="I56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="8:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H57" t="s">
         <v>45</v>
       </c>
-      <c r="I57" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H58" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H59" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H60" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="61" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I60" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H61" t="s">
         <v>49</v>
       </c>
-      <c r="I61" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H62" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="63" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I62" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H63" t="s">
         <v>51</v>
       </c>
-      <c r="I63" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H64" t="s">
         <v>52</v>
+      </c>
+      <c r="I64" t="s">
+        <v>55</v>
+      </c>
+      <c r="J64" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="65" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H65" t="s">
         <v>53</v>
       </c>
-      <c r="I65" t="s">
-        <v>56</v>
-      </c>
-      <c r="J65" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="66" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H66" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="67" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H67" t="s">
-        <v>55</v>
-      </c>
-      <c r="I67" t="s">
-        <v>56</v>
-      </c>
-      <c r="J67" t="s">
-        <v>56</v>
+      <c r="I66" t="s">
+        <v>55</v>
+      </c>
+      <c r="J66" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more different instance changes
</commit_message>
<xml_diff>
--- a/TilerElements/migrationStatus.xlsx
+++ b/TilerElements/migrationStatus.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6135" yWindow="0" windowWidth="56175" windowHeight="28995"/>
+    <workbookView xWindow="7065" yWindow="0" windowWidth="56175" windowHeight="28995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
   <si>
     <t>BlobSubCalendarEvent.cs</t>
   </si>
@@ -198,13 +198,23 @@
   </si>
   <si>
     <t>migrated</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,9 +243,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,420 +563,458 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H10:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="35.125" customWidth="1"/>
+    <col min="1" max="7" width="9" style="1"/>
+    <col min="8" max="8" width="35.125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="10" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H11" t="s">
+      <c r="H11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I11" t="s">
-        <v>55</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="I11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="12" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H12" t="s">
+      <c r="H12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I12" t="s">
-        <v>55</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="I12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="13" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H13" t="s">
+      <c r="H13" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H14" t="s">
+      <c r="H14" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H15" s="1">
+      <c r="H15" s="2">
         <v>42995</v>
       </c>
     </row>
     <row r="16" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H16" t="s">
+      <c r="H16" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H17" t="s">
+      <c r="H17" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H18" t="s">
+      <c r="H18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="19" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H19" t="s">
+      <c r="H19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I19" t="s">
-        <v>55</v>
-      </c>
-      <c r="J19" t="s">
+      <c r="I19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H20" t="s">
+      <c r="H20" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="I20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="21" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H21" t="s">
+      <c r="H21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I21" t="s">
-        <v>55</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="I21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="22" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H22" t="s">
+      <c r="H22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I22" t="s">
-        <v>55</v>
-      </c>
-      <c r="J22" t="s">
+      <c r="I22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="23" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H23" t="s">
+      <c r="H23" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="I23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="24" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H24" t="s">
+      <c r="H24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="25" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H25" t="s">
+      <c r="H25" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="I25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="26" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H26" t="s">
+      <c r="H26" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="I26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="27" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H27" t="s">
+      <c r="H27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I27" t="s">
-        <v>55</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="I27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="28" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H28" t="s">
+      <c r="H28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="29" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H29" t="s">
+      <c r="H29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I29" t="s">
-        <v>55</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="I29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="30" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H30" t="s">
+      <c r="H30" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="31" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H31" t="s">
+      <c r="H31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="32" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H32" t="s">
+      <c r="H32" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="33" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H33" t="s">
+      <c r="H33" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="34" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H34" t="s">
+      <c r="H34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="35" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H35" t="s">
+      <c r="H35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I35" t="s">
-        <v>55</v>
-      </c>
-      <c r="J35" t="s">
+      <c r="I35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="36" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H36" t="s">
+      <c r="H36" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="37" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H37" t="s">
+      <c r="H37" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="38" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H38" t="s">
+      <c r="H38" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="39" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H39" t="s">
+      <c r="H39" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="40" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H40" t="s">
+      <c r="H40" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="41" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H41" t="s">
+      <c r="H41" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="42" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H42" t="s">
+      <c r="H42" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="43" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H43" t="s">
+      <c r="H43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I43" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="44" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H44" t="s">
+      <c r="H44" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="45" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H45" t="s">
+      <c r="H45" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I45" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="46" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H46" t="s">
+      <c r="H46" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="47" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H47" t="s">
+      <c r="H47" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="48" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H48" t="s">
+      <c r="H48" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="49" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H49" t="s">
+      <c r="H49" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="50" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H50" t="s">
+      <c r="H50" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="51" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H51" t="s">
+      <c r="H51" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I51" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="52" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H52" t="s">
+      <c r="H52" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I52" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="53" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H53" t="s">
+      <c r="H53" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I53" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="54" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H54" t="s">
+      <c r="H54" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I54" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="55" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H55" t="s">
+      <c r="H55" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I55" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="56" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H56" t="s">
+      <c r="H56" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I56" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="57" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H57" t="s">
+      <c r="H57" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="58" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H58" t="s">
+      <c r="H58" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="59" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H59" t="s">
+      <c r="H59" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="60" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H60" t="s">
+      <c r="H60" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I60" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="61" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H61" t="s">
+      <c r="H61" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="62" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H62" t="s">
+      <c r="H62" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I62" t="s">
+      <c r="I62" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="63" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H63" t="s">
+      <c r="H63" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="64" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H64" t="s">
+      <c r="H64" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I64" t="s">
-        <v>55</v>
-      </c>
-      <c r="J64" t="s">
+      <c r="I64" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J64" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="65" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H65" t="s">
+      <c r="H65" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="66" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H66" t="s">
+      <c r="H66" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I66" t="s">
-        <v>55</v>
-      </c>
-      <c r="J66" t="s">
+      <c r="I66" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J66" s="1" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed pause profile and updated excel file
</commit_message>
<xml_diff>
--- a/TilerElements/migrationStatus.xlsx
+++ b/TilerElements/migrationStatus.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerom\Documents\Visual Studio 2015\Projects\WagTap\My24HourTimerWPF\TilerElements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerom\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7995" yWindow="0" windowWidth="56175" windowHeight="28995"/>
+    <workbookView xWindow="10785" yWindow="0" windowWidth="56175" windowHeight="28995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="60">
   <si>
     <t>BlobSubCalendarEvent.cs</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -563,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H10:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,10 +831,22 @@
       <c r="H36" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="I36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="37" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H37" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="8:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added procrastination to IUndoables
</commit_message>
<xml_diff>
--- a/TilerElements/migrationStatus.xlsx
+++ b/TilerElements/migrationStatus.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerom\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerom\Documents\Visual Studio 2015\Projects\WagTap\My24HourTimerWPF\TilerElements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10785" yWindow="0" windowWidth="56175" windowHeight="28995"/>
+    <workbookView xWindow="11715" yWindow="0" windowWidth="56175" windowHeight="28995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="60">
   <si>
     <t>BlobSubCalendarEvent.cs</t>
   </si>
@@ -246,10 +246,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H10:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,11 +862,20 @@
       <c r="I39" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="J39" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="40" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H40" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="I40" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="41" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H41" s="1" t="s">
@@ -873,6 +883,9 @@
       </c>
       <c r="I41" s="1" t="s">
         <v>55</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="8:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added every element to db and created undoables
</commit_message>
<xml_diff>
--- a/TilerElements/migrationStatus.xlsx
+++ b/TilerElements/migrationStatus.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11715" yWindow="0" windowWidth="56175" windowHeight="28995"/>
+    <workbookView xWindow="12645" yWindow="0" windowWidth="56175" windowHeight="28995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="61">
   <si>
     <t>BlobSubCalendarEvent.cs</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>ConflictProfile.cs</t>
   </si>
 </sst>
 </file>
@@ -567,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H10:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,26 +615,56 @@
       <c r="H13" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="I13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H14" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="I14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="15" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H15" s="2">
-        <v>42995</v>
+      <c r="H15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H16" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="I16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="17" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H17" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="18" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H18" s="1" t="s">
@@ -640,6 +673,9 @@
       <c r="I18" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="J18" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="19" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H19" s="1" t="s">
@@ -854,6 +890,12 @@
       <c r="H38" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="I38" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="39" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H39" s="1" t="s">
@@ -871,10 +913,10 @@
         <v>28</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="8:10" x14ac:dyDescent="0.25">
@@ -895,6 +937,9 @@
       <c r="I42" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="J42" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="43" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H43" s="1" t="s">
@@ -903,6 +948,9 @@
       <c r="I43" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="J43" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="44" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H44" s="1" t="s">
@@ -911,6 +959,9 @@
       <c r="I44" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="J44" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="45" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H45" s="1" t="s">
@@ -919,31 +970,64 @@
       <c r="I45" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="J45" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="46" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H46" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="I46" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="47" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H47" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="I47" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="48" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H48" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="I48" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="49" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H49" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="I49" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="50" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H50" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="I50" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="51" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H51" s="1" t="s">
@@ -952,6 +1036,9 @@
       <c r="I51" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="J51" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="52" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H52" s="1" t="s">
@@ -960,6 +1047,9 @@
       <c r="I52" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="J52" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="53" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H53" s="1" t="s">
@@ -968,6 +1058,9 @@
       <c r="I53" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="J53" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="54" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H54" s="1" t="s">
@@ -976,6 +1069,9 @@
       <c r="I54" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="J54" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="55" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H55" s="1" t="s">
@@ -984,6 +1080,9 @@
       <c r="I55" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="J55" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="56" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H56" s="1" t="s">
@@ -992,21 +1091,42 @@
       <c r="I56" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="J56" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="57" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H57" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="I57" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="58" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H58" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="I58" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="59" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H59" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="I59" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="60" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H60" s="1" t="s">
@@ -1020,6 +1140,12 @@
       <c r="H61" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="I61" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="62" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H62" s="1" t="s">
@@ -1028,11 +1154,20 @@
       <c r="I62" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="J62" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="63" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H63" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="I63" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="64" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H64" s="1" t="s">
@@ -1048,6 +1183,12 @@
     <row r="65" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H65" s="1" t="s">
         <v>53</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="8:10" x14ac:dyDescent="0.25">

</xml_diff>